<commit_message>
flow control in jupyter
</commit_message>
<xml_diff>
--- a/week2/data.xlsx
+++ b/week2/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sugarkhuu\Documents\python\repo\Introduction_Python\week2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE08F27-4A35-4BCF-827D-9A2BACBA7A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73294ED-E0E8-4CC0-8E47-7BD3AE8AD1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{489879BE-C2A9-4EAA-8795-529B20F48590}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,7 +879,7 @@
         <v>44013</v>
       </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>